<commit_message>
chore: update excel file.
</commit_message>
<xml_diff>
--- a/scenarios.xlsx
+++ b/scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOUFYANE\Desktop\Test&amp;Validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOUFYANE\Desktop\Test&amp;Validation\houta_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Titre du test</t>
   </si>
@@ -108,12 +108,21 @@
 - Un message d’information apparaît indiquant qu’aucun produit ne correspond à la recherche.
 </t>
   </si>
+  <si>
+    <t>AYOUB</t>
+  </si>
+  <si>
+    <t>ADIB</t>
+  </si>
+  <si>
+    <t>YOUNNES</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +164,23 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +190,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -178,11 +207,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -199,9 +229,13 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,14 +672,9 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -674,14 +703,16 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -818,14 +849,9 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
@@ -854,14 +880,16 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="C35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
@@ -989,14 +1017,16 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="21" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="C50" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
     </row>
     <row r="51" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
@@ -3375,6 +3405,11 @@
       <c r="G314" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C50:G50"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>